<commit_message>
WGP Zusammenfassung 1 Klausur
</commit_message>
<xml_diff>
--- a/Zwischenprüfung/Plan.xlsx
+++ b/Zwischenprüfung/Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Berufsschule\OriginSchule\Zwischenprüfung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FBA3BA-652A-4994-A4D3-D1B31CE4CDA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C98AB8D-2EB1-4B26-A99E-EEF60104367A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,18 +100,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -198,7 +193,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -278,7 +273,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -318,7 +313,7 @@
                   <a14:compatExt spid="_x0000_s1052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{553B5601-061C-4CB1-B478-3BA1DE7B9D69}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -385,7 +380,7 @@
                   <a14:compatExt spid="_x0000_s1053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3921AB45-FBEE-4047-980F-86142CCECDFC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -452,7 +447,7 @@
                   <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C14F475-A440-4C39-9F5C-B4FDF106AF8E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -519,7 +514,7 @@
                   <a14:compatExt spid="_x0000_s1055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE01D8CB-38B5-4B66-A204-49698A182483}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -586,7 +581,7 @@
                   <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B528C67B-61F1-43F4-972D-A9B5EB2D20A5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -653,7 +648,7 @@
                   <a14:compatExt spid="_x0000_s1057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7C18D7E-FCCE-476F-AEF8-5D8B8916AA8C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -720,7 +715,7 @@
                   <a14:compatExt spid="_x0000_s1058"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1B84773-AB52-4864-85F6-0841D0D70F25}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -787,7 +782,7 @@
                   <a14:compatExt spid="_x0000_s1059"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BA1F0C0-DE79-4469-9724-522C81BA2F7B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -854,7 +849,7 @@
                   <a14:compatExt spid="_x0000_s1060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AE31553-9CAA-466E-9B68-39889DE15855}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -921,7 +916,7 @@
                   <a14:compatExt spid="_x0000_s1061"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A8B72E9-296B-4E4A-B5FC-AE282CAC503D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -988,7 +983,7 @@
                   <a14:compatExt spid="_x0000_s1062"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3501A57-D177-49C7-8BD4-27D4F0A51F3E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1055,7 +1050,7 @@
                   <a14:compatExt spid="_x0000_s1063"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA7485FF-A288-47CB-BD6C-7229EB2F9F9E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1122,7 +1117,7 @@
                   <a14:compatExt spid="_x0000_s1064"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76F03F6A-1CB9-4B97-A768-B5D5054E5F94}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1189,7 +1184,7 @@
                   <a14:compatExt spid="_x0000_s1065"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65129FF7-D847-40BA-9422-DFAE6C4EE141}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1256,7 +1251,7 @@
                   <a14:compatExt spid="_x0000_s1066"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC039D7A-97DD-4A60-B873-3D3BC4D1CB7A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1323,7 +1318,7 @@
                   <a14:compatExt spid="_x0000_s1067"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29A96A4F-FB28-475C-B62E-4B076C977347}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1390,7 +1385,7 @@
                   <a14:compatExt spid="_x0000_s1068"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31D02E2D-5558-4C7F-871F-EBDFF1167CFE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1457,7 +1452,7 @@
                   <a14:compatExt spid="_x0000_s1069"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FBCCE57-964F-4F58-B6DD-5E0A8299C9A7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1524,7 +1519,7 @@
                   <a14:compatExt spid="_x0000_s1070"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C4CD428-86F6-4CB9-9C56-18DFC33F66DD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1591,7 +1586,7 @@
                   <a14:compatExt spid="_x0000_s1071"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13137AFC-A5DA-4CFD-B1BD-766386BD8085}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1658,7 +1653,7 @@
                   <a14:compatExt spid="_x0000_s1072"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E588DA78-5E4C-4C2E-98A7-664005AAC3F5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1725,7 +1720,7 @@
                   <a14:compatExt spid="_x0000_s1073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CA38B03-7D21-40CC-966A-7C586C3AA672}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1792,7 +1787,7 @@
                   <a14:compatExt spid="_x0000_s1074"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9976BD4-216F-45F9-93A9-31FDDDCE25CF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1859,7 +1854,7 @@
                   <a14:compatExt spid="_x0000_s1075"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BAFF605-82EB-422B-A0D4-A6FFE4314442}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1926,7 +1921,7 @@
                   <a14:compatExt spid="_x0000_s1076"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3A9ABFE-1EA1-40AD-87D3-6EC8F5C53567}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1993,7 +1988,7 @@
                   <a14:compatExt spid="_x0000_s1077"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EEF8862-8EEB-456C-BABC-FEA8251B9ECE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2060,7 +2055,7 @@
                   <a14:compatExt spid="_x0000_s1079"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC139A0D-10FC-4DB6-A7FA-DBCCFA9965B5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2127,7 +2122,7 @@
                   <a14:compatExt spid="_x0000_s1080"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BD88470-6966-446A-AC1E-8E57E67DE2D7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2194,7 +2189,7 @@
                   <a14:compatExt spid="_x0000_s1081"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E086FCD-1112-4238-9203-798E4EAE1C6B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2261,7 +2256,7 @@
                   <a14:compatExt spid="_x0000_s1082"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49711482-BD76-4946-BAFC-A8E6A7DC932B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2328,7 +2323,7 @@
                   <a14:compatExt spid="_x0000_s1083"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D14237A6-BC75-4D0E-AF04-CA4F142351EC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2395,7 +2390,7 @@
                   <a14:compatExt spid="_x0000_s1084"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{673B4C7C-8ABC-4074-BBA8-902A9AA5AB4D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2462,7 +2457,7 @@
                   <a14:compatExt spid="_x0000_s1085"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D9FFD0E-6197-440C-B511-3F2A0F85447A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2529,7 +2524,7 @@
                   <a14:compatExt spid="_x0000_s1086"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F3399B1-2B78-48AA-B595-DF7CB4634E99}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2596,7 +2591,7 @@
                   <a14:compatExt spid="_x0000_s1087"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8D50748-7E72-414A-8B33-A1FF8E221F1F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2909,7 +2904,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>